<commit_message>
[GEN MCU] SCH 수정, PL 작성
</commit_message>
<xml_diff>
--- a/1_LF_Generator_MCU/LF_Gen_Review Data_20171211.xlsx
+++ b/1_LF_Generator_MCU/LF_Gen_Review Data_20171211.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -89,6 +89,30 @@
   </si>
   <si>
     <t>Rdown</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ohm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -211,7 +235,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -246,7 +270,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -458,7 +482,7 @@
   <dimension ref="B3:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -523,15 +547,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:E7"/>
+  <dimension ref="B4:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -544,13 +568,16 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>4.7</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -558,8 +585,17 @@
       <c r="E5" t="s">
         <v>12</v>
       </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5">
+        <v>3.3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>14</v>
       </c>
@@ -572,14 +608,23 @@
       <c r="E6" t="s">
         <v>12</v>
       </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6">
+        <v>470</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7">
         <f>C4*C6/(C6+C5)</f>
-        <v>2.5</v>
+        <v>3.4013605442176873</v>
       </c>
       <c r="D7" s="4">
         <f>D4*D6/(D6+D5)</f>
@@ -587,6 +632,16 @@
       </c>
       <c r="E7" t="s">
         <v>9</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="4">
+        <f>I5/I6*1000</f>
+        <v>7.0212765957446797</v>
+      </c>
+      <c r="J7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>